<commit_message>
regression NN and ReadMe
</commit_message>
<xml_diff>
--- a/Summaries/parameters.xlsx
+++ b/Summaries/parameters.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="63">
   <si>
     <t>Model nr</t>
   </si>
   <si>
-    <t>test_size</t>
-  </si>
-  <si>
     <t>Normalise</t>
   </si>
   <si>
@@ -80,18 +77,9 @@
     <t>cat_crossentropy</t>
   </si>
   <si>
-    <t>optimizer</t>
-  </si>
-  <si>
     <t>adam</t>
   </si>
   <si>
-    <t>Class Num</t>
-  </si>
-  <si>
-    <t>Num hidden layers</t>
-  </si>
-  <si>
     <t>output layer</t>
   </si>
   <si>
@@ -131,9 +119,6 @@
     <t>RMSprop</t>
   </si>
   <si>
-    <t>Feature eng.</t>
-  </si>
-  <si>
     <t>Added types</t>
   </si>
   <si>
@@ -159,6 +144,75 @@
   </si>
   <si>
     <t>mean_squared_error</t>
+  </si>
+  <si>
+    <t>Kfold</t>
+  </si>
+  <si>
+    <t>val_mean_squared_error</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>dense 416</t>
+  </si>
+  <si>
+    <t>14(larger)</t>
+  </si>
+  <si>
+    <t>15(wider)</t>
+  </si>
+  <si>
+    <t>10Kfold</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>dense 20</t>
+  </si>
+  <si>
+    <t>dense 12</t>
+  </si>
+  <si>
+    <t>Dense 256</t>
+  </si>
+  <si>
+    <t>mean_absolute_error</t>
+  </si>
+  <si>
+    <t>Feat eng</t>
+  </si>
+  <si>
+    <t>Num clas</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>opt</t>
+  </si>
+  <si>
+    <t>Num hidden</t>
+  </si>
+  <si>
+    <t>Kfold mean score</t>
+  </si>
+  <si>
+    <t>13(standard)</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Accuracy test</t>
+  </si>
+  <si>
+    <t>Norm</t>
+  </si>
+  <si>
+    <t>act</t>
   </si>
 </sst>
 </file>
@@ -480,123 +534,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" customWidth="1"/>
     <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
       </c>
       <c r="E2">
         <v>0.3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
       </c>
       <c r="M2">
         <v>100</v>
@@ -605,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P2">
         <v>0.5</v>
@@ -621,41 +678,41 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
+      <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>0.3</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
       </c>
       <c r="M3">
         <v>800</v>
@@ -664,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P3">
         <v>0.54</v>
@@ -680,41 +737,41 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
+      <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>0.2</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M4">
         <v>15</v>
@@ -723,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="1">
         <v>0.66</v>
@@ -732,45 +789,45 @@
         <v>1E-3</v>
       </c>
       <c r="U4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M5">
         <v>5000</v>
@@ -779,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P5">
         <v>0.79</v>
@@ -790,41 +847,41 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6">
+      <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>0.2</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M6">
         <v>100</v>
@@ -833,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q6" s="1">
         <v>0.75</v>
@@ -842,45 +899,45 @@
         <v>1E-3</v>
       </c>
       <c r="U6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7">
+      <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>0.2</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H7">
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M7">
         <v>100</v>
@@ -889,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="1">
         <v>0.71</v>
@@ -898,45 +955,45 @@
         <v>1E-3</v>
       </c>
       <c r="U7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8">
+      <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>0.2</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H8">
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M8">
         <v>100</v>
@@ -945,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="1">
         <v>0.71</v>
@@ -954,39 +1011,39 @@
         <v>1E-3</v>
       </c>
       <c r="U8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9">
+      <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
       </c>
       <c r="E9">
         <v>0.2</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M9">
         <v>100</v>
@@ -995,51 +1052,51 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q9" s="1">
         <v>0.72615383068720496</v>
       </c>
       <c r="U9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M10">
         <v>5000</v>
@@ -1048,48 +1105,48 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q10" s="1">
         <v>79.7</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11">
+      <c r="A11">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>0.33</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M11">
         <v>50</v>
@@ -1098,95 +1155,466 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="1">
         <v>98.15</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="Q12" s="1"/>
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>11</v>
+      </c>
+      <c r="R12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
+      <c r="E13">
+        <v>0.3</v>
       </c>
       <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="S13">
+        <v>0.61499999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" t="s">
+        <v>57</v>
+      </c>
+      <c r="S14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13">
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
+        <v>47</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+      <c r="O15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15">
+        <v>0.54</v>
+      </c>
+      <c r="U15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="O16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16">
+        <v>0.53</v>
+      </c>
+      <c r="U16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+      <c r="O17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17">
+        <v>0.52</v>
+      </c>
+      <c r="U17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
-        <v>8</v>
-      </c>
-      <c r="M13">
-        <v>100</v>
-      </c>
-      <c r="O13" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q13" s="1"/>
-      <c r="R13">
-        <v>-0.54</v>
-      </c>
-      <c r="S13">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.3">
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="17:17" x14ac:dyDescent="0.3">
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="17:17" x14ac:dyDescent="0.3">
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19">
+        <v>500</v>
+      </c>
+      <c r="O19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="R19">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="Q29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>